<commit_message>
return path of report file
</commit_message>
<xml_diff>
--- a/weather_data.xlsx
+++ b/weather_data.xlsx
@@ -491,7 +491,7 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>45418.87087271651</v>
+        <v>45418.8718807485</v>
       </c>
       <c r="B2" t="n">
         <v>6.8</v>
@@ -522,12 +522,12 @@
         </is>
       </c>
       <c r="J2" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>45418.87122521962</v>
+        <v>45418.87223409885</v>
       </c>
       <c r="B3" t="n">
         <v>6.8</v>
@@ -558,29 +558,29 @@
         </is>
       </c>
       <c r="J3" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>45418.8718807485</v>
+        <v>45419.78927764975</v>
       </c>
       <c r="B4" t="n">
-        <v>6.8</v>
+        <v>3.7</v>
       </c>
       <c r="C4" t="n">
-        <v>2.38</v>
+        <v>3.18</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>WindDirection.NORTH_EAST</t>
+          <t>WindDirection.NORTH</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>989.8</v>
+        <v>988.8</v>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="G4" t="n">
         <v>0</v>
@@ -594,26 +594,26 @@
         </is>
       </c>
       <c r="J4" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>45418.87223409885</v>
+        <v>45419.82200312015</v>
       </c>
       <c r="B5" t="n">
-        <v>6.8</v>
+        <v>3.5</v>
       </c>
       <c r="C5" t="n">
-        <v>2.38</v>
+        <v>2.53</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>WindDirection.NORTH_EAST</t>
+          <t>WindDirection.NORTH</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>989.8</v>
+        <v>989.2</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
@@ -630,18 +630,18 @@
         </is>
       </c>
       <c r="J5" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>45419.78927764975</v>
+        <v>45419.82614997998</v>
       </c>
       <c r="B6" t="n">
-        <v>3.7</v>
+        <v>3.5</v>
       </c>
       <c r="C6" t="n">
-        <v>3.18</v>
+        <v>2.24</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -649,10 +649,10 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>988.8</v>
+        <v>989.3</v>
       </c>
       <c r="F6" t="n">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="G6" t="n">
         <v>0</v>
@@ -666,18 +666,18 @@
         </is>
       </c>
       <c r="J6" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>45419.82200312015</v>
+        <v>45419.82692761706</v>
       </c>
       <c r="B7" t="n">
         <v>3.5</v>
       </c>
       <c r="C7" t="n">
-        <v>2.53</v>
+        <v>2.24</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -685,7 +685,7 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>989.2</v>
+        <v>989.3</v>
       </c>
       <c r="F7" t="n">
         <v>0</v>
@@ -702,18 +702,18 @@
         </is>
       </c>
       <c r="J7" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>45419.82614997998</v>
+        <v>45419.83940991868</v>
       </c>
       <c r="B8" t="n">
-        <v>3.5</v>
+        <v>3.4</v>
       </c>
       <c r="C8" t="n">
-        <v>2.24</v>
+        <v>2.02</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -721,7 +721,7 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>989.3</v>
+        <v>989.4</v>
       </c>
       <c r="F8" t="n">
         <v>0</v>
@@ -738,18 +738,18 @@
         </is>
       </c>
       <c r="J8" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>45419.82692761706</v>
+        <v>45419.84608221337</v>
       </c>
       <c r="B9" t="n">
-        <v>3.5</v>
+        <v>3.3</v>
       </c>
       <c r="C9" t="n">
-        <v>2.24</v>
+        <v>1.65</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -757,7 +757,7 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>989.3</v>
+        <v>989.6</v>
       </c>
       <c r="F9" t="n">
         <v>0</v>
@@ -774,26 +774,26 @@
         </is>
       </c>
       <c r="J9" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>45419.83940991868</v>
+        <v>45419.86436986816</v>
       </c>
       <c r="B10" t="n">
-        <v>3.4</v>
+        <v>3.1</v>
       </c>
       <c r="C10" t="n">
-        <v>2.02</v>
+        <v>1.39</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>WindDirection.NORTH</t>
+          <t>WindDirection.NORTH_WEST</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>989.4</v>
+        <v>989.7</v>
       </c>
       <c r="F10" t="n">
         <v>0</v>
@@ -810,26 +810,26 @@
         </is>
       </c>
       <c r="J10" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>45419.84608221337</v>
+        <v>45419.86855657802</v>
       </c>
       <c r="B11" t="n">
-        <v>3.3</v>
+        <v>3</v>
       </c>
       <c r="C11" t="n">
-        <v>1.65</v>
+        <v>1.27</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>WindDirection.NORTH</t>
+          <t>WindDirection.NORTH_WEST</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>989.6</v>
+        <v>989.9</v>
       </c>
       <c r="F11" t="n">
         <v>0</v>
@@ -846,7 +846,7 @@
         </is>
       </c>
       <c r="J11" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>